<commit_message>
CalorimeterV4 update 2.2.1 gitignore
</commit_message>
<xml_diff>
--- a/strategy_test.xlsx
+++ b/strategy_test.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet name="Evaluation" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Raw_Data_COM" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Dia_Raw_Temp" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Dia_Raw_Voltage" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,16 +28,49 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor rgb="003BCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor rgb="003D33FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor rgb="00FF087F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightTrellis">
+        <fgColor rgb="003BCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightTrellis">
+        <fgColor rgb="003D33FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightTrellis">
+        <fgColor rgb="004B0082"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -43,18 +78,570 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick"/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Raw_Data_COM'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Raw_Data_COM'!$A$2:$A$32</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Raw_Data_COM'!$B$2:$B$32</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'Raw_Data_COM'!C1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Raw_Data_COM'!$A$2:$A$32</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Raw_Data_COM'!$C$2:$C$32</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <strRef>
+              <f>'Raw_Data_COM'!D1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Raw_Data_COM'!$A$2:$A$32</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Raw_Data_COM'!$D$2:$D$32</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <strRef>
+              <f>'Raw_Data_COM'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Raw_Data_COM'!$A$2:$A$32</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Raw_Data_COM'!$E$2:$E$32</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <strRef>
+              <f>'Raw_Data_COM'!F1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Raw_Data_COM'!$A$2:$A$32</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Raw_Data_COM'!$F$2:$F$32</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <strRef>
+              <f>'Raw_Data_COM'!G1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Raw_Data_COM'!$A$2:$A$32</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Raw_Data_COM'!$G$2:$G$32</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <tx>
+            <strRef>
+              <f>'Raw_Data_COM'!H1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Raw_Data_COM'!$A$2:$A$32</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Raw_Data_COM'!$H$2:$H$32</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Time [s]</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+        <tickLblSkip val="4"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Temperature [°C]</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Raw_Data_COM'!I1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Raw_Data_COM'!$A$2:$A$32</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Raw_Data_COM'!$I$2:$I$32</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'Raw_Data_COM'!J1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Raw_Data_COM'!$A$2:$A$32</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Raw_Data_COM'!$J$2:$J$32</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <strRef>
+              <f>'Raw_Data_COM'!K1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Raw_Data_COM'!$A$2:$A$32</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Raw_Data_COM'!$K$2:$K$32</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Time [s]</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+        <tickLblSkip val="4"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Voltage [mV]</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <absoluteAnchor>
+    <pos x="0" y="0"/>
+    <ext cx="0" cy="0"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </absoluteAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <absoluteAnchor>
+    <pos x="0" y="0"/>
+    <ext cx="0" cy="0"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </absoluteAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -355,87 +942,87 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Substance Data</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Substance</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Molar Mass [g/mol]</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>Weighing [g]</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>Volume [ml]</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>Concentration [mol/l]</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t>Additional data</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>a</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="3" t="n">
         <v>40.01</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="3" t="n">
         <v>250</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" s="3" t="n">
         <v>0.9997500624843789</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H3" s="4" t="inlineStr">
         <is>
           <t>concentration [mol/l]</t>
         </is>
       </c>
-      <c r="I3" t="n">
+      <c r="I3" s="5" t="n">
         <v>55.34276991396059</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="6" t="inlineStr">
         <is>
           <t>b</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="6" t="n">
         <v>60.05</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="6" t="n">
         <v>250</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" s="6" t="n">
         <v>0.9991673605328893</v>
       </c>
       <c r="H4" t="inlineStr">
@@ -443,69 +1030,69 @@
           <t>cp [J/(molK)]</t>
         </is>
       </c>
-      <c r="I4" t="n">
+      <c r="I4" s="7" t="n">
         <v>75.336</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>Process setup</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>Process Points</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>Evaluation Start Time</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>Evaluation End Time</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="2" t="inlineStr">
         <is>
           <t>V_A [ml/min]</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" s="2" t="inlineStr">
         <is>
           <t>V_A,act [ml/min]</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="2" t="inlineStr">
         <is>
           <t>n_A,act [mol/s]</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G7" s="2" t="inlineStr">
         <is>
           <t>n_A,act,water [mol/s]</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H7" s="2" t="inlineStr">
         <is>
           <t>V_B [ml/min]</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I7" s="2" t="inlineStr">
         <is>
           <t>V_B,act [ml/min]</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="J7" s="2" t="inlineStr">
         <is>
           <t>n_B,act [mol/s]</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="K7" s="2" t="inlineStr">
         <is>
           <t>n_B,act,water [mol/s]</t>
         </is>
@@ -519,12 +1106,12 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" s="8" t="n">
         <v>1</v>
       </c>
       <c r="F8" t="n">
@@ -536,7 +1123,7 @@
       <c r="H8" t="n">
         <v>1</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8" s="9" t="n">
         <v>1</v>
       </c>
       <c r="J8" t="n">
@@ -548,64 +1135,64 @@
     </row>
     <row r="9"/>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="1" t="inlineStr">
         <is>
           <t>Raw Data Processing</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>Process Points</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>T_A [°C]</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="2" t="inlineStr">
         <is>
           <t>T_B [°C]</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="2" t="inlineStr">
         <is>
           <t>T_out [°C]</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" s="2" t="inlineStr">
         <is>
           <t>Upre [V]</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" s="2" t="inlineStr">
         <is>
           <t>Ur1 [V]</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G11" s="2" t="inlineStr">
         <is>
           <t>Ur2 [V]</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="H11" s="2" t="inlineStr">
         <is>
           <t>dT_A [°C]</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="I11" s="2" t="inlineStr">
         <is>
           <t>dT_B [°C]</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="J11" s="2" t="inlineStr">
         <is>
           <t>dT_out [°C]</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="K11" s="2" t="inlineStr">
         <is>
           <t>Q_Out [W]</t>
         </is>
@@ -616,81 +1203,81 @@
         <v>1</v>
       </c>
       <c r="B12" t="n">
-        <v>15.52909090909091</v>
+        <v>15.6765</v>
       </c>
       <c r="C12" t="n">
-        <v>15.50090909090909</v>
+        <v>15.5145</v>
       </c>
       <c r="D12" t="n">
-        <v>15.44545454545454</v>
+        <v>15.4085</v>
       </c>
       <c r="E12" t="n">
-        <v>15.48454545454546</v>
+        <v>15.432</v>
       </c>
       <c r="F12" t="n">
-        <v>15.47272727272727</v>
+        <v>15.4225</v>
       </c>
       <c r="G12" t="n">
-        <v>14.9</v>
+        <v>14.885</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.5290909090909111</v>
+        <v>-0.6764999999999954</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.5009090909090901</v>
+        <v>-0.5144999999999982</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.4454545454545435</v>
+        <v>-0.4085000000000001</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.0619078311508084</v>
+        <v>-0.05677200801554261</v>
       </c>
     </row>
     <row r="13"/>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="1" t="inlineStr">
         <is>
           <t>Calculation</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="2" t="inlineStr">
         <is>
           <t>Process Points</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>Q_A [W]</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="2" t="inlineStr">
         <is>
           <t>Q_B [W]</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" s="2" t="inlineStr">
         <is>
           <t>Qpre [W] - cp flux</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E15" s="2" t="inlineStr">
         <is>
           <t>QSE,pre [W]</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" s="2" t="inlineStr">
         <is>
           <t>Qr1 [W]</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G15" s="2" t="inlineStr">
         <is>
           <t>Qr2 [W]</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="H15" s="2" t="inlineStr">
         <is>
           <t>dHr [kJ/mol]</t>
         </is>
@@ -701,28 +1288,35 @@
         <v>1</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.03676567115282733</v>
+        <v>-0.04700889035803466</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.03480736220826073</v>
+        <v>-0.03575177248959188</v>
       </c>
       <c r="D16" t="n">
-        <v>-273.7402388429753</v>
+        <v>-272.010624</v>
       </c>
       <c r="E16" t="n">
-        <v>-273.6686658096142</v>
+        <v>-271.9278633371523</v>
       </c>
       <c r="F16" t="n">
-        <v>-273.3507438016529</v>
+        <v>-271.69850625</v>
       </c>
       <c r="G16" t="n">
-        <v>-254.81</v>
-      </c>
-      <c r="H16" t="n">
-        <v>-48153.57361241719</v>
+        <v>-254.333225</v>
+      </c>
+      <c r="H16" s="10" t="n">
+        <v>-47920.88281403982</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -733,7 +1327,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC23"/>
+  <dimension ref="A1:AC32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -896,31 +1490,31 @@
         <v>14.55</v>
       </c>
       <c r="C2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D2" t="n">
         <v>15.15</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>14.55</v>
       </c>
-      <c r="E2" t="n">
-        <v>15</v>
-      </c>
       <c r="F2" t="n">
-        <v>15.39</v>
+        <v>15.54</v>
       </c>
       <c r="G2" t="n">
-        <v>15.6</v>
+        <v>15.76</v>
       </c>
       <c r="H2" t="n">
-        <v>15.5</v>
+        <v>15.65</v>
       </c>
       <c r="I2" t="n">
-        <v>15.04</v>
+        <v>15.35</v>
       </c>
       <c r="J2" t="n">
-        <v>15.19</v>
+        <v>15.65</v>
       </c>
       <c r="K2" t="n">
-        <v>14.45</v>
+        <v>14.9</v>
       </c>
       <c r="L2" t="n">
         <v>-0.02</v>
@@ -944,10 +1538,10 @@
         <v>-4.08</v>
       </c>
       <c r="S2" t="n">
-        <v>-3.06</v>
+        <v>-3.03</v>
       </c>
       <c r="T2" t="n">
-        <v>-0.98</v>
+        <v>-1</v>
       </c>
       <c r="U2" t="n">
         <v>0</v>
@@ -959,13 +1553,13 @@
         <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>-3.96</v>
+        <v>-4</v>
       </c>
       <c r="Y2" t="n">
-        <v>-3.06</v>
+        <v>-2.94</v>
       </c>
       <c r="Z2" t="n">
-        <v>-1.02</v>
+        <v>-1.01</v>
       </c>
       <c r="AA2" t="n">
         <v>0</v>
@@ -982,34 +1576,34 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>15.15</v>
+        <v>14.55</v>
       </c>
       <c r="C3" t="n">
+        <v>14.55</v>
+      </c>
+      <c r="D3" t="n">
+        <v>14.85</v>
+      </c>
+      <c r="E3" t="n">
         <v>15</v>
       </c>
-      <c r="D3" t="n">
-        <v>15</v>
-      </c>
-      <c r="E3" t="n">
-        <v>14.55</v>
-      </c>
       <c r="F3" t="n">
-        <v>15.23</v>
+        <v>15.39</v>
       </c>
       <c r="G3" t="n">
         <v>15.29</v>
       </c>
       <c r="H3" t="n">
-        <v>15.65</v>
+        <v>15.04</v>
       </c>
       <c r="I3" t="n">
-        <v>15.65</v>
+        <v>15.35</v>
       </c>
       <c r="J3" t="n">
-        <v>15.35</v>
+        <v>15.5</v>
       </c>
       <c r="K3" t="n">
-        <v>14.45</v>
+        <v>14.9</v>
       </c>
       <c r="L3" t="n">
         <v>-0.02</v>
@@ -1033,10 +1627,10 @@
         <v>-4.04</v>
       </c>
       <c r="S3" t="n">
-        <v>-3</v>
+        <v>-3.03</v>
       </c>
       <c r="T3" t="n">
-        <v>-0.99</v>
+        <v>-0.97</v>
       </c>
       <c r="U3" t="n">
         <v>0</v>
@@ -1048,13 +1642,13 @@
         <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>-3.88</v>
+        <v>-4.08</v>
       </c>
       <c r="Y3" t="n">
         <v>-2.91</v>
       </c>
       <c r="Z3" t="n">
-        <v>-0.97</v>
+        <v>-1</v>
       </c>
       <c r="AA3" t="n">
         <v>0</v>
@@ -1071,7 +1665,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>15</v>
+        <v>14.7</v>
       </c>
       <c r="C4" t="n">
         <v>14.85</v>
@@ -1080,31 +1674,31 @@
         <v>14.55</v>
       </c>
       <c r="E4" t="n">
-        <v>14.55</v>
+        <v>15</v>
       </c>
       <c r="F4" t="n">
-        <v>15.86</v>
+        <v>15.7</v>
       </c>
       <c r="G4" t="n">
         <v>15.91</v>
       </c>
       <c r="H4" t="n">
-        <v>15.19</v>
+        <v>15.04</v>
       </c>
       <c r="I4" t="n">
         <v>15.65</v>
       </c>
       <c r="J4" t="n">
-        <v>15.35</v>
+        <v>15.04</v>
       </c>
       <c r="K4" t="n">
-        <v>14.45</v>
+        <v>15.2</v>
       </c>
       <c r="L4" t="n">
         <v>-0.02</v>
       </c>
       <c r="M4" t="n">
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
       <c r="N4" t="n">
         <v>0.04</v>
@@ -1122,7 +1716,7 @@
         <v>-3.96</v>
       </c>
       <c r="S4" t="n">
-        <v>-3.03</v>
+        <v>-3</v>
       </c>
       <c r="T4" t="n">
         <v>-1.01</v>
@@ -1137,10 +1731,10 @@
         <v>0</v>
       </c>
       <c r="X4" t="n">
-        <v>-3.88</v>
+        <v>-4</v>
       </c>
       <c r="Y4" t="n">
-        <v>-2.97</v>
+        <v>-3.03</v>
       </c>
       <c r="Z4" t="n">
         <v>-1.01</v>
@@ -1160,40 +1754,40 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="C5" t="n">
         <v>14.85</v>
       </c>
-      <c r="C5" t="n">
-        <v>15</v>
-      </c>
       <c r="D5" t="n">
-        <v>14.7</v>
+        <v>15.15</v>
       </c>
       <c r="E5" t="n">
         <v>14.7</v>
       </c>
       <c r="F5" t="n">
-        <v>15.7</v>
+        <v>15.86</v>
       </c>
       <c r="G5" t="n">
-        <v>15.6</v>
+        <v>15.29</v>
       </c>
       <c r="H5" t="n">
-        <v>15.04</v>
+        <v>15.19</v>
       </c>
       <c r="I5" t="n">
-        <v>15.35</v>
+        <v>15.5</v>
       </c>
       <c r="J5" t="n">
         <v>15.81</v>
       </c>
       <c r="K5" t="n">
-        <v>15.05</v>
+        <v>14.9</v>
       </c>
       <c r="L5" t="n">
         <v>-0.02</v>
       </c>
       <c r="M5" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="N5" t="n">
         <v>0.04</v>
@@ -1208,13 +1802,13 @@
         <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>-3.96</v>
+        <v>-3.88</v>
       </c>
       <c r="S5" t="n">
         <v>-3.03</v>
       </c>
       <c r="T5" t="n">
-        <v>-1.02</v>
+        <v>-0.98</v>
       </c>
       <c r="U5" t="n">
         <v>0</v>
@@ -1226,13 +1820,13 @@
         <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>-3.96</v>
+        <v>-4.04</v>
       </c>
       <c r="Y5" t="n">
-        <v>-3.06</v>
+        <v>-2.94</v>
       </c>
       <c r="Z5" t="n">
-        <v>-0.99</v>
+        <v>-1.01</v>
       </c>
       <c r="AA5" t="n">
         <v>0</v>
@@ -1252,37 +1846,37 @@
         <v>14.55</v>
       </c>
       <c r="C6" t="n">
-        <v>14.85</v>
+        <v>14.55</v>
       </c>
       <c r="D6" t="n">
-        <v>14.7</v>
+        <v>15.15</v>
       </c>
       <c r="E6" t="n">
-        <v>15.15</v>
+        <v>15.3</v>
       </c>
       <c r="F6" t="n">
         <v>15.23</v>
       </c>
       <c r="G6" t="n">
-        <v>15.76</v>
+        <v>15.6</v>
       </c>
       <c r="H6" t="n">
-        <v>15.04</v>
+        <v>15.81</v>
       </c>
       <c r="I6" t="n">
-        <v>15.04</v>
+        <v>15.35</v>
       </c>
       <c r="J6" t="n">
-        <v>15.65</v>
+        <v>15.5</v>
       </c>
       <c r="K6" t="n">
-        <v>14.6</v>
+        <v>14.75</v>
       </c>
       <c r="L6" t="n">
         <v>-0.02</v>
       </c>
       <c r="M6" t="n">
-        <v>0.44</v>
+        <v>0.46</v>
       </c>
       <c r="N6" t="n">
         <v>0.04</v>
@@ -1297,13 +1891,13 @@
         <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>-4.08</v>
+        <v>-3.88</v>
       </c>
       <c r="S6" t="n">
         <v>-3</v>
       </c>
       <c r="T6" t="n">
-        <v>-1.01</v>
+        <v>-1</v>
       </c>
       <c r="U6" t="n">
         <v>0</v>
@@ -1318,10 +1912,10 @@
         <v>-3.92</v>
       </c>
       <c r="Y6" t="n">
-        <v>-2.91</v>
+        <v>-3.03</v>
       </c>
       <c r="Z6" t="n">
-        <v>-0.99</v>
+        <v>-1.01</v>
       </c>
       <c r="AA6" t="n">
         <v>0</v>
@@ -1338,40 +1932,40 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
+        <v>14.55</v>
+      </c>
+      <c r="C7" t="n">
+        <v>14.55</v>
+      </c>
+      <c r="D7" t="n">
         <v>15</v>
       </c>
-      <c r="C7" t="n">
-        <v>15</v>
-      </c>
-      <c r="D7" t="n">
-        <v>15.3</v>
-      </c>
       <c r="E7" t="n">
-        <v>14.55</v>
+        <v>15.15</v>
       </c>
       <c r="F7" t="n">
-        <v>15.7</v>
+        <v>15.23</v>
       </c>
       <c r="G7" t="n">
-        <v>15.6</v>
+        <v>15.76</v>
       </c>
       <c r="H7" t="n">
-        <v>15.65</v>
+        <v>15.19</v>
       </c>
       <c r="I7" t="n">
-        <v>15.35</v>
+        <v>15.04</v>
       </c>
       <c r="J7" t="n">
-        <v>15.35</v>
+        <v>15.5</v>
       </c>
       <c r="K7" t="n">
-        <v>14.9</v>
+        <v>15.2</v>
       </c>
       <c r="L7" t="n">
         <v>-0.02</v>
       </c>
       <c r="M7" t="n">
-        <v>0.46</v>
+        <v>0.45</v>
       </c>
       <c r="N7" t="n">
         <v>0.04</v>
@@ -1386,7 +1980,7 @@
         <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>-3.96</v>
+        <v>-4.04</v>
       </c>
       <c r="S7" t="n">
         <v>-3.03</v>
@@ -1404,13 +1998,13 @@
         <v>0</v>
       </c>
       <c r="X7" t="n">
-        <v>-3.96</v>
+        <v>-3.88</v>
       </c>
       <c r="Y7" t="n">
-        <v>-3</v>
+        <v>-3.06</v>
       </c>
       <c r="Z7" t="n">
-        <v>-1</v>
+        <v>-1.01</v>
       </c>
       <c r="AA7" t="n">
         <v>0</v>
@@ -1427,34 +2021,34 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>15</v>
+        <v>15.15</v>
       </c>
       <c r="C8" t="n">
-        <v>15</v>
+        <v>14.55</v>
       </c>
       <c r="D8" t="n">
-        <v>14.55</v>
+        <v>14.85</v>
       </c>
       <c r="E8" t="n">
-        <v>14.85</v>
+        <v>14.7</v>
       </c>
       <c r="F8" t="n">
-        <v>15.7</v>
+        <v>16.01</v>
       </c>
       <c r="G8" t="n">
-        <v>15.6</v>
+        <v>15.13</v>
       </c>
       <c r="H8" t="n">
-        <v>15.81</v>
+        <v>15.04</v>
       </c>
       <c r="I8" t="n">
-        <v>15.5</v>
+        <v>15.35</v>
       </c>
       <c r="J8" t="n">
         <v>15.35</v>
       </c>
       <c r="K8" t="n">
-        <v>14.45</v>
+        <v>15.05</v>
       </c>
       <c r="L8" t="n">
         <v>-0.02</v>
@@ -1475,13 +2069,13 @@
         <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>-3.92</v>
+        <v>-4</v>
       </c>
       <c r="S8" t="n">
         <v>-2.94</v>
       </c>
       <c r="T8" t="n">
-        <v>-1.02</v>
+        <v>-0.97</v>
       </c>
       <c r="U8" t="n">
         <v>0</v>
@@ -1493,13 +2087,13 @@
         <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>-3.92</v>
+        <v>-3.88</v>
       </c>
       <c r="Y8" t="n">
-        <v>-3.06</v>
+        <v>-3</v>
       </c>
       <c r="Z8" t="n">
-        <v>-0.97</v>
+        <v>-0.99</v>
       </c>
       <c r="AA8" t="n">
         <v>0</v>
@@ -1516,40 +2110,40 @@
         <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>15</v>
+        <v>14.55</v>
       </c>
       <c r="C9" t="n">
-        <v>15.15</v>
+        <v>15.3</v>
       </c>
       <c r="D9" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="E9" t="n">
         <v>14.85</v>
       </c>
-      <c r="E9" t="n">
-        <v>15.15</v>
-      </c>
       <c r="F9" t="n">
-        <v>15.39</v>
+        <v>15.7</v>
       </c>
       <c r="G9" t="n">
-        <v>15.6</v>
+        <v>15.29</v>
       </c>
       <c r="H9" t="n">
         <v>15.5</v>
       </c>
       <c r="I9" t="n">
-        <v>15.35</v>
+        <v>15.5</v>
       </c>
       <c r="J9" t="n">
-        <v>15.81</v>
+        <v>15.5</v>
       </c>
       <c r="K9" t="n">
-        <v>15.2</v>
+        <v>14.45</v>
       </c>
       <c r="L9" t="n">
         <v>-0.02</v>
       </c>
       <c r="M9" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="N9" t="n">
         <v>0.04</v>
@@ -1564,7 +2158,7 @@
         <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>-3.92</v>
+        <v>-4.04</v>
       </c>
       <c r="S9" t="n">
         <v>-2.91</v>
@@ -1582,13 +2176,13 @@
         <v>0</v>
       </c>
       <c r="X9" t="n">
-        <v>-3.88</v>
+        <v>-4.04</v>
       </c>
       <c r="Y9" t="n">
-        <v>-3</v>
+        <v>-2.91</v>
       </c>
       <c r="Z9" t="n">
-        <v>-0.98</v>
+        <v>-0.99</v>
       </c>
       <c r="AA9" t="n">
         <v>0</v>
@@ -1605,31 +2199,31 @@
         <v>13</v>
       </c>
       <c r="B10" t="n">
-        <v>14.7</v>
+        <v>15</v>
       </c>
       <c r="C10" t="n">
-        <v>14.7</v>
+        <v>14.85</v>
       </c>
       <c r="D10" t="n">
         <v>14.55</v>
       </c>
       <c r="E10" t="n">
-        <v>15.15</v>
+        <v>14.85</v>
       </c>
       <c r="F10" t="n">
-        <v>15.86</v>
+        <v>15.7</v>
       </c>
       <c r="G10" t="n">
-        <v>15.44</v>
+        <v>15.29</v>
       </c>
       <c r="H10" t="n">
-        <v>15.81</v>
+        <v>15.5</v>
       </c>
       <c r="I10" t="n">
-        <v>15.5</v>
+        <v>15.04</v>
       </c>
       <c r="J10" t="n">
-        <v>15.35</v>
+        <v>15.65</v>
       </c>
       <c r="K10" t="n">
         <v>15.2</v>
@@ -1638,7 +2232,7 @@
         <v>-0.02</v>
       </c>
       <c r="M10" t="n">
-        <v>0.46</v>
+        <v>0.45</v>
       </c>
       <c r="N10" t="n">
         <v>0.04</v>
@@ -1653,31 +2247,31 @@
         <v>0</v>
       </c>
       <c r="R10" t="n">
-        <v>-3.88</v>
+        <v>-3.96</v>
       </c>
       <c r="S10" t="n">
-        <v>-2.97</v>
+        <v>-2.91</v>
       </c>
       <c r="T10" t="n">
+        <v>-1.02</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0</v>
+      </c>
+      <c r="X10" t="n">
+        <v>-4.04</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>-3.06</v>
+      </c>
+      <c r="Z10" t="n">
         <v>-1</v>
-      </c>
-      <c r="U10" t="n">
-        <v>0</v>
-      </c>
-      <c r="V10" t="n">
-        <v>0</v>
-      </c>
-      <c r="W10" t="n">
-        <v>0</v>
-      </c>
-      <c r="X10" t="n">
-        <v>-3.92</v>
-      </c>
-      <c r="Y10" t="n">
-        <v>-2.97</v>
-      </c>
-      <c r="Z10" t="n">
-        <v>-0.97</v>
       </c>
       <c r="AA10" t="n">
         <v>0</v>
@@ -1694,40 +2288,40 @@
         <v>14</v>
       </c>
       <c r="B11" t="n">
+        <v>14.85</v>
+      </c>
+      <c r="C11" t="n">
         <v>14.55</v>
       </c>
-      <c r="C11" t="n">
-        <v>15</v>
-      </c>
       <c r="D11" t="n">
-        <v>15.15</v>
+        <v>14.7</v>
       </c>
       <c r="E11" t="n">
-        <v>15.15</v>
+        <v>14.55</v>
       </c>
       <c r="F11" t="n">
-        <v>15.86</v>
+        <v>15.7</v>
       </c>
       <c r="G11" t="n">
-        <v>15.44</v>
+        <v>15.91</v>
       </c>
       <c r="H11" t="n">
+        <v>15.35</v>
+      </c>
+      <c r="I11" t="n">
+        <v>15.19</v>
+      </c>
+      <c r="J11" t="n">
         <v>15.65</v>
       </c>
-      <c r="I11" t="n">
-        <v>15.81</v>
-      </c>
-      <c r="J11" t="n">
-        <v>15.35</v>
-      </c>
       <c r="K11" t="n">
-        <v>14.9</v>
+        <v>15.2</v>
       </c>
       <c r="L11" t="n">
         <v>-0.02</v>
       </c>
       <c r="M11" t="n">
-        <v>0.46</v>
+        <v>0.45</v>
       </c>
       <c r="N11" t="n">
         <v>0.04</v>
@@ -1742,13 +2336,13 @@
         <v>0</v>
       </c>
       <c r="R11" t="n">
-        <v>-4.08</v>
+        <v>-3.92</v>
       </c>
       <c r="S11" t="n">
-        <v>-3</v>
+        <v>-2.97</v>
       </c>
       <c r="T11" t="n">
-        <v>-0.99</v>
+        <v>-1.02</v>
       </c>
       <c r="U11" t="n">
         <v>0</v>
@@ -1760,13 +2354,13 @@
         <v>0</v>
       </c>
       <c r="X11" t="n">
-        <v>-3.96</v>
+        <v>-3.88</v>
       </c>
       <c r="Y11" t="n">
-        <v>-2.91</v>
+        <v>-3.03</v>
       </c>
       <c r="Z11" t="n">
-        <v>-1.01</v>
+        <v>-1</v>
       </c>
       <c r="AA11" t="n">
         <v>0</v>
@@ -1783,34 +2377,34 @@
         <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>14.85</v>
+        <v>15.3</v>
       </c>
       <c r="C12" t="n">
-        <v>14.55</v>
+        <v>15.15</v>
       </c>
       <c r="D12" t="n">
-        <v>14.7</v>
+        <v>15.15</v>
       </c>
       <c r="E12" t="n">
-        <v>14.55</v>
+        <v>15.3</v>
       </c>
       <c r="F12" t="n">
-        <v>15.7</v>
+        <v>16.01</v>
       </c>
       <c r="G12" t="n">
-        <v>15.76</v>
+        <v>15.13</v>
       </c>
       <c r="H12" t="n">
+        <v>15.81</v>
+      </c>
+      <c r="I12" t="n">
+        <v>15.35</v>
+      </c>
+      <c r="J12" t="n">
         <v>15.04</v>
       </c>
-      <c r="I12" t="n">
-        <v>15.19</v>
-      </c>
-      <c r="J12" t="n">
-        <v>15.5</v>
-      </c>
       <c r="K12" t="n">
-        <v>14.9</v>
+        <v>14.45</v>
       </c>
       <c r="L12" t="n">
         <v>-0.02</v>
@@ -1831,10 +2425,10 @@
         <v>0</v>
       </c>
       <c r="R12" t="n">
-        <v>-3.92</v>
+        <v>-4.04</v>
       </c>
       <c r="S12" t="n">
-        <v>-3</v>
+        <v>-3.06</v>
       </c>
       <c r="T12" t="n">
         <v>-1.02</v>
@@ -1849,13 +2443,13 @@
         <v>0</v>
       </c>
       <c r="X12" t="n">
-        <v>-4.04</v>
+        <v>-4.08</v>
       </c>
       <c r="Y12" t="n">
-        <v>-3.06</v>
+        <v>-2.91</v>
       </c>
       <c r="Z12" t="n">
-        <v>-0.98</v>
+        <v>-1.02</v>
       </c>
       <c r="AA12" t="n">
         <v>0</v>
@@ -1872,40 +2466,40 @@
         <v>16</v>
       </c>
       <c r="B13" t="n">
-        <v>15.3</v>
+        <v>14.85</v>
       </c>
       <c r="C13" t="n">
-        <v>14.85</v>
+        <v>15.15</v>
       </c>
       <c r="D13" t="n">
-        <v>15.3</v>
+        <v>14.55</v>
       </c>
       <c r="E13" t="n">
-        <v>15.3</v>
+        <v>14.55</v>
       </c>
       <c r="F13" t="n">
-        <v>15.23</v>
+        <v>15.86</v>
       </c>
       <c r="G13" t="n">
-        <v>15.76</v>
+        <v>15.13</v>
       </c>
       <c r="H13" t="n">
-        <v>15.5</v>
+        <v>15.04</v>
       </c>
       <c r="I13" t="n">
-        <v>15.04</v>
+        <v>15.35</v>
       </c>
       <c r="J13" t="n">
         <v>15.35</v>
       </c>
       <c r="K13" t="n">
-        <v>14.9</v>
+        <v>14.45</v>
       </c>
       <c r="L13" t="n">
         <v>-0.02</v>
       </c>
       <c r="M13" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="N13" t="n">
         <v>0.04</v>
@@ -1920,31 +2514,31 @@
         <v>0</v>
       </c>
       <c r="R13" t="n">
+        <v>-4</v>
+      </c>
+      <c r="S13" t="n">
+        <v>-2.97</v>
+      </c>
+      <c r="T13" t="n">
+        <v>-1.02</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0</v>
+      </c>
+      <c r="X13" t="n">
         <v>-3.92</v>
       </c>
-      <c r="S13" t="n">
+      <c r="Y13" t="n">
         <v>-2.91</v>
       </c>
-      <c r="T13" t="n">
-        <v>-1</v>
-      </c>
-      <c r="U13" t="n">
-        <v>0</v>
-      </c>
-      <c r="V13" t="n">
-        <v>0</v>
-      </c>
-      <c r="W13" t="n">
-        <v>0</v>
-      </c>
-      <c r="X13" t="n">
-        <v>-4.08</v>
-      </c>
-      <c r="Y13" t="n">
-        <v>-2.97</v>
-      </c>
       <c r="Z13" t="n">
-        <v>-1.02</v>
+        <v>-0.99</v>
       </c>
       <c r="AA13" t="n">
         <v>0</v>
@@ -1964,31 +2558,31 @@
         <v>15</v>
       </c>
       <c r="C14" t="n">
-        <v>14.7</v>
+        <v>15.15</v>
       </c>
       <c r="D14" t="n">
         <v>14.55</v>
       </c>
       <c r="E14" t="n">
-        <v>14.55</v>
+        <v>14.85</v>
       </c>
       <c r="F14" t="n">
         <v>15.54</v>
       </c>
       <c r="G14" t="n">
-        <v>15.6</v>
+        <v>15.91</v>
       </c>
       <c r="H14" t="n">
+        <v>15.35</v>
+      </c>
+      <c r="I14" t="n">
         <v>15.5</v>
       </c>
-      <c r="I14" t="n">
-        <v>15.19</v>
-      </c>
       <c r="J14" t="n">
-        <v>15.04</v>
+        <v>15.65</v>
       </c>
       <c r="K14" t="n">
-        <v>14.9</v>
+        <v>14.75</v>
       </c>
       <c r="L14" t="n">
         <v>-0.02</v>
@@ -2009,13 +2603,13 @@
         <v>0</v>
       </c>
       <c r="R14" t="n">
-        <v>-3.92</v>
+        <v>-3.88</v>
       </c>
       <c r="S14" t="n">
-        <v>-2.94</v>
+        <v>-3.06</v>
       </c>
       <c r="T14" t="n">
-        <v>-1.01</v>
+        <v>-1</v>
       </c>
       <c r="U14" t="n">
         <v>0</v>
@@ -2027,13 +2621,13 @@
         <v>0</v>
       </c>
       <c r="X14" t="n">
-        <v>-3.96</v>
+        <v>-4</v>
       </c>
       <c r="Y14" t="n">
-        <v>-2.97</v>
+        <v>-3</v>
       </c>
       <c r="Z14" t="n">
-        <v>-0.99</v>
+        <v>-1</v>
       </c>
       <c r="AA14" t="n">
         <v>0</v>
@@ -2053,7 +2647,7 @@
         <v>15</v>
       </c>
       <c r="C15" t="n">
-        <v>15.3</v>
+        <v>14.55</v>
       </c>
       <c r="D15" t="n">
         <v>14.55</v>
@@ -2065,16 +2659,16 @@
         <v>15.54</v>
       </c>
       <c r="G15" t="n">
-        <v>15.44</v>
+        <v>15.76</v>
       </c>
       <c r="H15" t="n">
         <v>15.5</v>
       </c>
       <c r="I15" t="n">
-        <v>15.65</v>
+        <v>15.04</v>
       </c>
       <c r="J15" t="n">
-        <v>15.65</v>
+        <v>15.19</v>
       </c>
       <c r="K15" t="n">
         <v>14.9</v>
@@ -2104,7 +2698,7 @@
         <v>-2.91</v>
       </c>
       <c r="T15" t="n">
-        <v>-1.01</v>
+        <v>-1.02</v>
       </c>
       <c r="U15" t="n">
         <v>0</v>
@@ -2116,13 +2710,13 @@
         <v>0</v>
       </c>
       <c r="X15" t="n">
-        <v>-4</v>
+        <v>-3.96</v>
       </c>
       <c r="Y15" t="n">
-        <v>-2.97</v>
+        <v>-3.03</v>
       </c>
       <c r="Z15" t="n">
-        <v>-1.02</v>
+        <v>-0.99</v>
       </c>
       <c r="AA15" t="n">
         <v>0</v>
@@ -2139,40 +2733,40 @@
         <v>19</v>
       </c>
       <c r="B16" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="C16" t="n">
+        <v>15.15</v>
+      </c>
+      <c r="D16" t="n">
         <v>14.55</v>
       </c>
-      <c r="C16" t="n">
-        <v>15.3</v>
-      </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>14.7</v>
       </c>
-      <c r="E16" t="n">
-        <v>14.55</v>
-      </c>
       <c r="F16" t="n">
-        <v>15.86</v>
+        <v>15.23</v>
       </c>
       <c r="G16" t="n">
-        <v>15.6</v>
+        <v>15.13</v>
       </c>
       <c r="H16" t="n">
+        <v>15.04</v>
+      </c>
+      <c r="I16" t="n">
         <v>15.5</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>15.65</v>
       </c>
-      <c r="J16" t="n">
-        <v>15.35</v>
-      </c>
       <c r="K16" t="n">
-        <v>14.6</v>
+        <v>14.75</v>
       </c>
       <c r="L16" t="n">
         <v>-0.02</v>
       </c>
       <c r="M16" t="n">
-        <v>0.44</v>
+        <v>0.46</v>
       </c>
       <c r="N16" t="n">
         <v>0.04</v>
@@ -2187,10 +2781,10 @@
         <v>0</v>
       </c>
       <c r="R16" t="n">
-        <v>-4</v>
+        <v>-3.92</v>
       </c>
       <c r="S16" t="n">
-        <v>-3.03</v>
+        <v>-3.06</v>
       </c>
       <c r="T16" t="n">
         <v>-1.02</v>
@@ -2205,13 +2799,13 @@
         <v>0</v>
       </c>
       <c r="X16" t="n">
-        <v>-3.96</v>
+        <v>-4.04</v>
       </c>
       <c r="Y16" t="n">
-        <v>-2.91</v>
+        <v>-2.97</v>
       </c>
       <c r="Z16" t="n">
-        <v>-1.02</v>
+        <v>-1.01</v>
       </c>
       <c r="AA16" t="n">
         <v>0</v>
@@ -2234,34 +2828,34 @@
         <v>14.85</v>
       </c>
       <c r="D17" t="n">
-        <v>15.15</v>
+        <v>14.7</v>
       </c>
       <c r="E17" t="n">
         <v>14.85</v>
       </c>
       <c r="F17" t="n">
-        <v>15.54</v>
+        <v>15.23</v>
       </c>
       <c r="G17" t="n">
-        <v>15.6</v>
+        <v>15.44</v>
       </c>
       <c r="H17" t="n">
-        <v>15.5</v>
+        <v>15.04</v>
       </c>
       <c r="I17" t="n">
         <v>15.81</v>
       </c>
       <c r="J17" t="n">
-        <v>15.65</v>
+        <v>15.5</v>
       </c>
       <c r="K17" t="n">
-        <v>15.2</v>
+        <v>14.6</v>
       </c>
       <c r="L17" t="n">
         <v>-0.02</v>
       </c>
       <c r="M17" t="n">
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
       <c r="N17" t="n">
         <v>0.04</v>
@@ -2276,13 +2870,13 @@
         <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>-3.92</v>
+        <v>-3.88</v>
       </c>
       <c r="S17" t="n">
         <v>-3.06</v>
       </c>
       <c r="T17" t="n">
-        <v>-0.98</v>
+        <v>-1.01</v>
       </c>
       <c r="U17" t="n">
         <v>0</v>
@@ -2294,13 +2888,13 @@
         <v>0</v>
       </c>
       <c r="X17" t="n">
-        <v>-3.96</v>
+        <v>-3.92</v>
       </c>
       <c r="Y17" t="n">
-        <v>-2.97</v>
+        <v>-2.94</v>
       </c>
       <c r="Z17" t="n">
-        <v>-0.97</v>
+        <v>-1.01</v>
       </c>
       <c r="AA17" t="n">
         <v>0</v>
@@ -2317,10 +2911,10 @@
         <v>21</v>
       </c>
       <c r="B18" t="n">
-        <v>15.15</v>
+        <v>14.7</v>
       </c>
       <c r="C18" t="n">
-        <v>14.85</v>
+        <v>15</v>
       </c>
       <c r="D18" t="n">
         <v>14.7</v>
@@ -2332,16 +2926,16 @@
         <v>15.7</v>
       </c>
       <c r="G18" t="n">
-        <v>15.13</v>
+        <v>15.76</v>
       </c>
       <c r="H18" t="n">
-        <v>15.81</v>
+        <v>15.5</v>
       </c>
       <c r="I18" t="n">
-        <v>15.65</v>
+        <v>15.35</v>
       </c>
       <c r="J18" t="n">
-        <v>15.81</v>
+        <v>15.04</v>
       </c>
       <c r="K18" t="n">
         <v>14.75</v>
@@ -2365,13 +2959,13 @@
         <v>0</v>
       </c>
       <c r="R18" t="n">
-        <v>-3.92</v>
+        <v>-3.88</v>
       </c>
       <c r="S18" t="n">
-        <v>-2.91</v>
+        <v>-3</v>
       </c>
       <c r="T18" t="n">
-        <v>-0.97</v>
+        <v>-0.99</v>
       </c>
       <c r="U18" t="n">
         <v>0</v>
@@ -2386,10 +2980,10 @@
         <v>-3.96</v>
       </c>
       <c r="Y18" t="n">
-        <v>-2.97</v>
+        <v>-3.06</v>
       </c>
       <c r="Z18" t="n">
-        <v>-1.02</v>
+        <v>-1</v>
       </c>
       <c r="AA18" t="n">
         <v>0</v>
@@ -2406,40 +3000,40 @@
         <v>22</v>
       </c>
       <c r="B19" t="n">
+        <v>15.15</v>
+      </c>
+      <c r="C19" t="n">
+        <v>15</v>
+      </c>
+      <c r="D19" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="E19" t="n">
         <v>14.85</v>
       </c>
-      <c r="C19" t="n">
-        <v>14.55</v>
-      </c>
-      <c r="D19" t="n">
-        <v>15.15</v>
-      </c>
-      <c r="E19" t="n">
-        <v>14.55</v>
-      </c>
       <c r="F19" t="n">
-        <v>15.23</v>
+        <v>15.7</v>
       </c>
       <c r="G19" t="n">
-        <v>15.76</v>
+        <v>15.13</v>
       </c>
       <c r="H19" t="n">
-        <v>15.81</v>
+        <v>15.35</v>
       </c>
       <c r="I19" t="n">
-        <v>15.04</v>
+        <v>15.35</v>
       </c>
       <c r="J19" t="n">
         <v>15.35</v>
       </c>
       <c r="K19" t="n">
-        <v>14.6</v>
+        <v>14.9</v>
       </c>
       <c r="L19" t="n">
         <v>-0.02</v>
       </c>
       <c r="M19" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="N19" t="n">
         <v>0.04</v>
@@ -2454,13 +3048,13 @@
         <v>0</v>
       </c>
       <c r="R19" t="n">
-        <v>-4.04</v>
+        <v>-4</v>
       </c>
       <c r="S19" t="n">
-        <v>-3</v>
+        <v>-3.03</v>
       </c>
       <c r="T19" t="n">
-        <v>-1.02</v>
+        <v>-0.99</v>
       </c>
       <c r="U19" t="n">
         <v>0</v>
@@ -2472,10 +3066,10 @@
         <v>0</v>
       </c>
       <c r="X19" t="n">
-        <v>-3.96</v>
+        <v>-3.88</v>
       </c>
       <c r="Y19" t="n">
-        <v>-2.97</v>
+        <v>-2.94</v>
       </c>
       <c r="Z19" t="n">
         <v>-1.01</v>
@@ -2498,28 +3092,28 @@
         <v>14.55</v>
       </c>
       <c r="C20" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="D20" t="n">
         <v>14.85</v>
-      </c>
-      <c r="D20" t="n">
-        <v>15.15</v>
       </c>
       <c r="E20" t="n">
         <v>14.85</v>
       </c>
       <c r="F20" t="n">
-        <v>15.86</v>
+        <v>15.54</v>
       </c>
       <c r="G20" t="n">
-        <v>15.13</v>
+        <v>15.6</v>
       </c>
       <c r="H20" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="I20" t="n">
+        <v>15.35</v>
+      </c>
+      <c r="J20" t="n">
         <v>15.04</v>
-      </c>
-      <c r="I20" t="n">
-        <v>15.19</v>
-      </c>
-      <c r="J20" t="n">
-        <v>15.81</v>
       </c>
       <c r="K20" t="n">
         <v>15.2</v>
@@ -2528,7 +3122,7 @@
         <v>-0.02</v>
       </c>
       <c r="M20" t="n">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
       <c r="N20" t="n">
         <v>0.04</v>
@@ -2543,13 +3137,13 @@
         <v>0</v>
       </c>
       <c r="R20" t="n">
-        <v>-3.96</v>
+        <v>-4</v>
       </c>
       <c r="S20" t="n">
         <v>-3</v>
       </c>
       <c r="T20" t="n">
-        <v>-1</v>
+        <v>-0.98</v>
       </c>
       <c r="U20" t="n">
         <v>0</v>
@@ -2561,10 +3155,10 @@
         <v>0</v>
       </c>
       <c r="X20" t="n">
-        <v>-4.04</v>
+        <v>-3.92</v>
       </c>
       <c r="Y20" t="n">
-        <v>-3</v>
+        <v>-2.97</v>
       </c>
       <c r="Z20" t="n">
         <v>-1.02</v>
@@ -2584,34 +3178,34 @@
         <v>24</v>
       </c>
       <c r="B21" t="n">
-        <v>15.15</v>
+        <v>14.7</v>
       </c>
       <c r="C21" t="n">
-        <v>14.55</v>
+        <v>14.85</v>
       </c>
       <c r="D21" t="n">
-        <v>14.55</v>
+        <v>14.85</v>
       </c>
       <c r="E21" t="n">
-        <v>14.85</v>
+        <v>14.7</v>
       </c>
       <c r="F21" t="n">
-        <v>15.23</v>
+        <v>15.86</v>
       </c>
       <c r="G21" t="n">
         <v>15.29</v>
       </c>
       <c r="H21" t="n">
-        <v>15.35</v>
+        <v>15.19</v>
       </c>
       <c r="I21" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="J21" t="n">
         <v>15.65</v>
       </c>
-      <c r="J21" t="n">
-        <v>15.19</v>
-      </c>
       <c r="K21" t="n">
-        <v>14.6</v>
+        <v>15.05</v>
       </c>
       <c r="L21" t="n">
         <v>-0.02</v>
@@ -2632,31 +3226,31 @@
         <v>0</v>
       </c>
       <c r="R21" t="n">
+        <v>-3.96</v>
+      </c>
+      <c r="S21" t="n">
+        <v>-2.94</v>
+      </c>
+      <c r="T21" t="n">
+        <v>-0.98</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V21" t="n">
+        <v>0</v>
+      </c>
+      <c r="W21" t="n">
+        <v>0</v>
+      </c>
+      <c r="X21" t="n">
         <v>-3.88</v>
       </c>
-      <c r="S21" t="n">
-        <v>-2.91</v>
-      </c>
-      <c r="T21" t="n">
+      <c r="Y21" t="n">
+        <v>-3.06</v>
+      </c>
+      <c r="Z21" t="n">
         <v>-0.99</v>
-      </c>
-      <c r="U21" t="n">
-        <v>0</v>
-      </c>
-      <c r="V21" t="n">
-        <v>0</v>
-      </c>
-      <c r="W21" t="n">
-        <v>0</v>
-      </c>
-      <c r="X21" t="n">
-        <v>-4</v>
-      </c>
-      <c r="Y21" t="n">
-        <v>-2.97</v>
-      </c>
-      <c r="Z21" t="n">
-        <v>-0.98</v>
       </c>
       <c r="AA21" t="n">
         <v>0</v>
@@ -2673,31 +3267,31 @@
         <v>25</v>
       </c>
       <c r="B22" t="n">
-        <v>15</v>
+        <v>14.85</v>
       </c>
       <c r="C22" t="n">
-        <v>14.55</v>
+        <v>14.7</v>
       </c>
       <c r="D22" t="n">
-        <v>14.7</v>
+        <v>14.85</v>
       </c>
       <c r="E22" t="n">
-        <v>15</v>
+        <v>15.15</v>
       </c>
       <c r="F22" t="n">
-        <v>15.86</v>
+        <v>15.39</v>
       </c>
       <c r="G22" t="n">
-        <v>15.29</v>
+        <v>15.76</v>
       </c>
       <c r="H22" t="n">
-        <v>15.35</v>
+        <v>15.81</v>
       </c>
       <c r="I22" t="n">
-        <v>15.81</v>
+        <v>15.19</v>
       </c>
       <c r="J22" t="n">
-        <v>15.81</v>
+        <v>15.65</v>
       </c>
       <c r="K22" t="n">
         <v>15.2</v>
@@ -2721,13 +3315,13 @@
         <v>0</v>
       </c>
       <c r="R22" t="n">
-        <v>-3.92</v>
+        <v>-4</v>
       </c>
       <c r="S22" t="n">
-        <v>-3.03</v>
+        <v>-2.97</v>
       </c>
       <c r="T22" t="n">
-        <v>-0.98</v>
+        <v>-1</v>
       </c>
       <c r="U22" t="n">
         <v>0</v>
@@ -2742,10 +3336,10 @@
         <v>-3.96</v>
       </c>
       <c r="Y22" t="n">
-        <v>-3.03</v>
+        <v>-3.06</v>
       </c>
       <c r="Z22" t="n">
-        <v>-0.98</v>
+        <v>-1.01</v>
       </c>
       <c r="AA22" t="n">
         <v>0</v>
@@ -2762,34 +3356,34 @@
         <v>26</v>
       </c>
       <c r="B23" t="n">
+        <v>15.15</v>
+      </c>
+      <c r="C23" t="n">
+        <v>14.55</v>
+      </c>
+      <c r="D23" t="n">
         <v>15.3</v>
       </c>
-      <c r="C23" t="n">
-        <v>14.7</v>
-      </c>
-      <c r="D23" t="n">
-        <v>14.7</v>
-      </c>
       <c r="E23" t="n">
-        <v>14.7</v>
+        <v>15.15</v>
       </c>
       <c r="F23" t="n">
-        <v>15.23</v>
+        <v>15.86</v>
       </c>
       <c r="G23" t="n">
-        <v>15.91</v>
+        <v>15.76</v>
       </c>
       <c r="H23" t="n">
-        <v>15.04</v>
+        <v>15.81</v>
       </c>
       <c r="I23" t="n">
+        <v>15.81</v>
+      </c>
+      <c r="J23" t="n">
         <v>15.65</v>
       </c>
-      <c r="J23" t="n">
-        <v>15.19</v>
-      </c>
       <c r="K23" t="n">
-        <v>15.05</v>
+        <v>15.2</v>
       </c>
       <c r="L23" t="n">
         <v>-0.02</v>
@@ -2810,39 +3404,840 @@
         <v>0</v>
       </c>
       <c r="R23" t="n">
+        <v>-3.88</v>
+      </c>
+      <c r="S23" t="n">
+        <v>-3.06</v>
+      </c>
+      <c r="T23" t="n">
+        <v>-1</v>
+      </c>
+      <c r="U23" t="n">
+        <v>0</v>
+      </c>
+      <c r="V23" t="n">
+        <v>0</v>
+      </c>
+      <c r="W23" t="n">
+        <v>0</v>
+      </c>
+      <c r="X23" t="n">
+        <v>-4.04</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>-2.97</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>-0.98</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>27</v>
+      </c>
+      <c r="B24" t="n">
+        <v>14.85</v>
+      </c>
+      <c r="C24" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="D24" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="E24" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="F24" t="n">
+        <v>15.54</v>
+      </c>
+      <c r="G24" t="n">
+        <v>15.29</v>
+      </c>
+      <c r="H24" t="n">
+        <v>15.19</v>
+      </c>
+      <c r="I24" t="n">
+        <v>15.04</v>
+      </c>
+      <c r="J24" t="n">
+        <v>15.65</v>
+      </c>
+      <c r="K24" t="n">
+        <v>14.9</v>
+      </c>
+      <c r="L24" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="n">
+        <v>-4.08</v>
+      </c>
+      <c r="S24" t="n">
+        <v>-3.06</v>
+      </c>
+      <c r="T24" t="n">
+        <v>-1</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V24" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" t="n">
+        <v>0</v>
+      </c>
+      <c r="X24" t="n">
+        <v>-3.88</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>-2.94</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>-1.01</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>28</v>
+      </c>
+      <c r="B25" t="n">
+        <v>14.85</v>
+      </c>
+      <c r="C25" t="n">
+        <v>14.85</v>
+      </c>
+      <c r="D25" t="n">
+        <v>15.15</v>
+      </c>
+      <c r="E25" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="F25" t="n">
+        <v>15.86</v>
+      </c>
+      <c r="G25" t="n">
+        <v>15.76</v>
+      </c>
+      <c r="H25" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="I25" t="n">
+        <v>15.81</v>
+      </c>
+      <c r="J25" t="n">
+        <v>15.35</v>
+      </c>
+      <c r="K25" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="L25" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" t="n">
+        <v>-3.92</v>
+      </c>
+      <c r="S25" t="n">
+        <v>-2.97</v>
+      </c>
+      <c r="T25" t="n">
+        <v>-1.01</v>
+      </c>
+      <c r="U25" t="n">
+        <v>0</v>
+      </c>
+      <c r="V25" t="n">
+        <v>0</v>
+      </c>
+      <c r="W25" t="n">
+        <v>0</v>
+      </c>
+      <c r="X25" t="n">
         <v>-4</v>
       </c>
-      <c r="S23" t="n">
+      <c r="Y25" t="n">
+        <v>-2.91</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>-0.99</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>29</v>
+      </c>
+      <c r="B26" t="n">
+        <v>15</v>
+      </c>
+      <c r="C26" t="n">
+        <v>15.15</v>
+      </c>
+      <c r="D26" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="E26" t="n">
+        <v>15</v>
+      </c>
+      <c r="F26" t="n">
+        <v>16.01</v>
+      </c>
+      <c r="G26" t="n">
+        <v>15.76</v>
+      </c>
+      <c r="H26" t="n">
+        <v>15.04</v>
+      </c>
+      <c r="I26" t="n">
+        <v>15.04</v>
+      </c>
+      <c r="J26" t="n">
+        <v>15.65</v>
+      </c>
+      <c r="K26" t="n">
+        <v>14.6</v>
+      </c>
+      <c r="L26" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" t="n">
+        <v>-3.96</v>
+      </c>
+      <c r="S26" t="n">
+        <v>-3.03</v>
+      </c>
+      <c r="T26" t="n">
+        <v>-1</v>
+      </c>
+      <c r="U26" t="n">
+        <v>0</v>
+      </c>
+      <c r="V26" t="n">
+        <v>0</v>
+      </c>
+      <c r="W26" t="n">
+        <v>0</v>
+      </c>
+      <c r="X26" t="n">
+        <v>-4.04</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>-2.91</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>-0.99</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>30</v>
+      </c>
+      <c r="B27" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="C27" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="D27" t="n">
+        <v>15.15</v>
+      </c>
+      <c r="E27" t="n">
+        <v>15</v>
+      </c>
+      <c r="F27" t="n">
+        <v>16.01</v>
+      </c>
+      <c r="G27" t="n">
+        <v>15.91</v>
+      </c>
+      <c r="H27" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="I27" t="n">
+        <v>15.19</v>
+      </c>
+      <c r="J27" t="n">
+        <v>15.04</v>
+      </c>
+      <c r="K27" t="n">
+        <v>14.6</v>
+      </c>
+      <c r="L27" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" t="n">
+        <v>-4.08</v>
+      </c>
+      <c r="S27" t="n">
         <v>-2.94</v>
       </c>
-      <c r="T23" t="n">
+      <c r="T27" t="n">
+        <v>-1.01</v>
+      </c>
+      <c r="U27" t="n">
+        <v>0</v>
+      </c>
+      <c r="V27" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" t="n">
+        <v>0</v>
+      </c>
+      <c r="X27" t="n">
+        <v>-3.96</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>-2.97</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>-0.97</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>31</v>
+      </c>
+      <c r="B28" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="C28" t="n">
+        <v>14.55</v>
+      </c>
+      <c r="D28" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="E28" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="F28" t="n">
+        <v>16.01</v>
+      </c>
+      <c r="G28" t="n">
+        <v>15.29</v>
+      </c>
+      <c r="H28" t="n">
+        <v>15.65</v>
+      </c>
+      <c r="I28" t="n">
+        <v>15.81</v>
+      </c>
+      <c r="J28" t="n">
+        <v>15.04</v>
+      </c>
+      <c r="K28" t="n">
+        <v>15.05</v>
+      </c>
+      <c r="L28" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" t="n">
+        <v>-4.08</v>
+      </c>
+      <c r="S28" t="n">
+        <v>-3.03</v>
+      </c>
+      <c r="T28" t="n">
         <v>-0.98</v>
       </c>
-      <c r="U23" t="n">
-        <v>0</v>
-      </c>
-      <c r="V23" t="n">
-        <v>0</v>
-      </c>
-      <c r="W23" t="n">
-        <v>0</v>
-      </c>
-      <c r="X23" t="n">
+      <c r="U28" t="n">
+        <v>0</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" t="n">
+        <v>0</v>
+      </c>
+      <c r="X28" t="n">
+        <v>-3.88</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>-3.03</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>-0.97</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32</v>
+      </c>
+      <c r="B29" t="n">
+        <v>15</v>
+      </c>
+      <c r="C29" t="n">
+        <v>14.55</v>
+      </c>
+      <c r="D29" t="n">
+        <v>14.85</v>
+      </c>
+      <c r="E29" t="n">
+        <v>15</v>
+      </c>
+      <c r="F29" t="n">
+        <v>15.86</v>
+      </c>
+      <c r="G29" t="n">
+        <v>15.44</v>
+      </c>
+      <c r="H29" t="n">
+        <v>15.81</v>
+      </c>
+      <c r="I29" t="n">
+        <v>15.65</v>
+      </c>
+      <c r="J29" t="n">
+        <v>15.65</v>
+      </c>
+      <c r="K29" t="n">
+        <v>15.05</v>
+      </c>
+      <c r="L29" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" t="n">
+        <v>-4</v>
+      </c>
+      <c r="S29" t="n">
+        <v>-2.94</v>
+      </c>
+      <c r="T29" t="n">
+        <v>-1</v>
+      </c>
+      <c r="U29" t="n">
+        <v>0</v>
+      </c>
+      <c r="V29" t="n">
+        <v>0</v>
+      </c>
+      <c r="W29" t="n">
+        <v>0</v>
+      </c>
+      <c r="X29" t="n">
+        <v>-3.96</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>-2.91</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>-0.99</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>33</v>
+      </c>
+      <c r="B30" t="n">
+        <v>14.55</v>
+      </c>
+      <c r="C30" t="n">
+        <v>14.85</v>
+      </c>
+      <c r="D30" t="n">
+        <v>14.85</v>
+      </c>
+      <c r="E30" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="F30" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="G30" t="n">
+        <v>15.6</v>
+      </c>
+      <c r="H30" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="I30" t="n">
+        <v>15.35</v>
+      </c>
+      <c r="J30" t="n">
+        <v>15.19</v>
+      </c>
+      <c r="K30" t="n">
+        <v>15.05</v>
+      </c>
+      <c r="L30" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" t="n">
         <v>-3.92</v>
       </c>
-      <c r="Y23" t="n">
+      <c r="S30" t="n">
+        <v>-3.06</v>
+      </c>
+      <c r="T30" t="n">
+        <v>-1</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0</v>
+      </c>
+      <c r="V30" t="n">
+        <v>0</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0</v>
+      </c>
+      <c r="X30" t="n">
+        <v>-3.92</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>-3</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>-0.99</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>34</v>
+      </c>
+      <c r="B31" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="C31" t="n">
+        <v>14.85</v>
+      </c>
+      <c r="D31" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="E31" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="F31" t="n">
+        <v>15.39</v>
+      </c>
+      <c r="G31" t="n">
+        <v>15.13</v>
+      </c>
+      <c r="H31" t="n">
+        <v>15.35</v>
+      </c>
+      <c r="I31" t="n">
+        <v>15.65</v>
+      </c>
+      <c r="J31" t="n">
+        <v>15.81</v>
+      </c>
+      <c r="K31" t="n">
+        <v>15.05</v>
+      </c>
+      <c r="L31" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" t="n">
+        <v>-3.88</v>
+      </c>
+      <c r="S31" t="n">
+        <v>-3.03</v>
+      </c>
+      <c r="T31" t="n">
+        <v>-0.97</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0</v>
+      </c>
+      <c r="V31" t="n">
+        <v>0</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0</v>
+      </c>
+      <c r="X31" t="n">
+        <v>-4.04</v>
+      </c>
+      <c r="Y31" t="n">
         <v>-2.94</v>
       </c>
-      <c r="Z23" t="n">
-        <v>-0.97</v>
-      </c>
-      <c r="AA23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC23" t="n">
+      <c r="Z31" t="n">
+        <v>-0.98</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>35</v>
+      </c>
+      <c r="B32" t="n">
+        <v>14.85</v>
+      </c>
+      <c r="C32" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="D32" t="n">
+        <v>15.15</v>
+      </c>
+      <c r="E32" t="n">
+        <v>14.85</v>
+      </c>
+      <c r="F32" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="G32" t="n">
+        <v>15.44</v>
+      </c>
+      <c r="H32" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="I32" t="n">
+        <v>15.35</v>
+      </c>
+      <c r="J32" t="n">
+        <v>15.35</v>
+      </c>
+      <c r="K32" t="n">
+        <v>14.45</v>
+      </c>
+      <c r="L32" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" t="n">
+        <v>-3.92</v>
+      </c>
+      <c r="S32" t="n">
+        <v>-2.94</v>
+      </c>
+      <c r="T32" t="n">
+        <v>-1</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0</v>
+      </c>
+      <c r="X32" t="n">
+        <v>-4.08</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>-3</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC32" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>